<commit_message>
pushing a couple updates
</commit_message>
<xml_diff>
--- a/2017 processed/Journal of Educational Psychology.xlsx
+++ b/2017 processed/Journal of Educational Psychology.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="460" windowWidth="25600" windowHeight="13940"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Journal of Educational Psych" sheetId="7" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="139">
   <si>
     <t>Type</t>
   </si>
@@ -379,9 +379,6 @@
     <t>Working memory strategies during rational number magnitude processing</t>
   </si>
   <si>
-    <t xml:space="preserve">no? but also remove some people for being 3sd away from the mean at one point </t>
-  </si>
-  <si>
     <t>Phonological processing in children with specific reading disorder versus typical learners: Factor structure and measurement invariance in a transparent orthography</t>
   </si>
   <si>
@@ -529,6 +526,18 @@
   </si>
   <si>
     <t>SEM models</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>At the group level, participants
+who scored below chance on the comparison task (n _x0002_ 2) or who
+had RTs greater than three standard deviations away from the
+group RT performance (n _x0002_ 2) were excluded</t>
   </si>
 </sst>
 </file>
@@ -656,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -691,6 +700,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1002,29 +1015,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F20" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="112.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="71.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="41.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="10"/>
+    <col min="16" max="16" width="11" style="17"/>
+    <col min="17" max="17" width="11" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1517,10 +1518,10 @@
         <v>79</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H15" s="22" t="s">
         <v>34</v>
@@ -1669,33 +1670,48 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="14"/>
     </row>
-    <row r="21" spans="1:18" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="21">
+    <row r="21" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="26">
         <v>15</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="22" t="s">
+      <c r="B21" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="27">
+        <v>60</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="N21" s="27">
         <v>57</v>
       </c>
-      <c r="H21" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="P21" s="24"/>
-      <c r="R21" s="25"/>
+      <c r="P21" s="28"/>
+      <c r="R21" s="29"/>
     </row>
     <row r="22" spans="1:18" s="22" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
@@ -1708,19 +1724,34 @@
         <v>43</v>
       </c>
       <c r="D22" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="23" t="s">
-        <v>95</v>
-      </c>
       <c r="F22" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G22" s="22">
         <v>209</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>108</v>
+        <v>136</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="N22" s="22">
+        <v>209</v>
       </c>
       <c r="P22" s="24"/>
       <c r="R22" s="25"/>
@@ -1736,13 +1767,13 @@
         <v>43</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G23" s="4">
         <v>4215</v>
@@ -1761,19 +1792,19 @@
         <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E24" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="G24" s="6">
         <v>245</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P24" s="16"/>
       <c r="R24" s="14"/>
@@ -1789,13 +1820,13 @@
         <v>43</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="G25" s="4">
         <v>141</v>
@@ -1817,13 +1848,13 @@
         <v>43</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="F26" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="G26" s="6">
         <v>115</v>
@@ -1846,13 +1877,13 @@
         <v>43</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>112</v>
-      </c>
       <c r="F27" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G27" s="4">
         <v>536</v>
@@ -1874,19 +1905,19 @@
         <v>43</v>
       </c>
       <c r="D28" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>114</v>
-      </c>
       <c r="F28" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G28" s="6">
         <v>153</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>38</v>
@@ -1898,7 +1929,7 @@
         <v>22</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M28" s="6" t="s">
         <v>41</v>
@@ -1918,16 +1949,16 @@
         <v>43</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F29" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>34</v>
@@ -1946,31 +1977,31 @@
         <v>43</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G30" s="6">
         <v>1420</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>40</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>41</v>
@@ -1979,7 +2010,7 @@
         <v>39</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P30" s="16"/>
       <c r="R30" s="14"/>
@@ -1995,16 +2026,16 @@
         <v>43</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>34</v>

</xml_diff>